<commit_message>
[CORRECTION] Corrige une typo dans le fichier template
</commit_message>
<xml_diff>
--- a/public/assets/fichiers/Template services - MSS.xlsx
+++ b/public/assets/fichiers/Template services - MSS.xlsx
@@ -41,7 +41,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ce fichier vous ai fournit par MonServiceSécurisé</t>
+      <t xml:space="preserve">Ce fichier vous est fourni par MonServiceSécurisé</t>
     </r>
   </si>
   <si>
@@ -478,9 +478,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1929600</xdr:colOff>
+      <xdr:colOff>1928880</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>815040</xdr:rowOff>
+      <xdr:rowOff>814320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -494,7 +494,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1929600" cy="815040"/>
+          <a:ext cx="1928880" cy="814320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -516,11 +516,11 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.35"/>

</xml_diff>